<commit_message>
Code Merge Changes - 9/25/2017
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite Statutory Adoption PaternityPay201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite Statutory Adoption PaternityPay201718.xlsx
@@ -1,30 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XCDHR\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="8" firstSheet="6" windowHeight="5400" windowWidth="15168" xWindow="384" yWindow="36"/>
+    <workbookView xWindow="390" yWindow="30" windowWidth="15165" windowHeight="5400" firstSheet="8" activeTab="10"/>
   </bookViews>
   <sheets>
-    <sheet name="first" r:id="rId1" sheetId="1"/>
-    <sheet name="ResetData" r:id="rId2" sheetId="14"/>
-    <sheet name="CreateFemaleEmployee" r:id="rId3" sheetId="2"/>
-    <sheet name="UpdateTaxCodeAndAnnualSalary" r:id="rId4" sheetId="6"/>
-    <sheet name="SmallEmployerRelief" r:id="rId5" sheetId="3"/>
-    <sheet name="ProcessPayrollForJulyMonthSAPP" r:id="rId6" sheetId="7"/>
-    <sheet name="ProcessPayrollForAugMonthSAPP" r:id="rId7" sheetId="8"/>
-    <sheet name="ProcessPayrollForSepMonthSAPP" r:id="rId8" sheetId="9"/>
-    <sheet name="CreateLeaveRequest" r:id="rId9" sheetId="10"/>
-    <sheet name="AverageWeeklyEarningsTestReport" r:id="rId10" sheetId="11"/>
-    <sheet name="ProcessPayrollForJan16MonthSAPP" r:id="rId11" sheetId="12"/>
+    <sheet name="first" sheetId="1" r:id="rId1"/>
+    <sheet name="ResetData" sheetId="14" r:id="rId2"/>
+    <sheet name="CreateFemaleEmployee" sheetId="2" r:id="rId3"/>
+    <sheet name="UpdateTaxCodeAndAnnualSalary" sheetId="6" r:id="rId4"/>
+    <sheet name="SmallEmployerRelief" sheetId="3" r:id="rId5"/>
+    <sheet name="ProcessPayrollForJulyMonthSAPP" sheetId="7" r:id="rId6"/>
+    <sheet name="ProcessPayrollForAugMonthSAPP" sheetId="8" r:id="rId7"/>
+    <sheet name="ProcessPayrollForSepMonthSAPP" sheetId="9" r:id="rId8"/>
+    <sheet name="CreateLeaveRequest" sheetId="10" r:id="rId9"/>
+    <sheet name="AverageWeeklyEarningsTestReport" sheetId="11" r:id="rId10"/>
+    <sheet name="ProcessPayrollForJan16MonthSAPP" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="186">
   <si>
     <t>TC</t>
   </si>
@@ -542,9 +547,6 @@
     <t>Payroll Suite Statutory Adoption PaternityPay201718.xlsx</t>
   </si>
   <si>
-    <t>F:\\Automation NI Reports\\HMRCTestData\Statutory scenarios for 201718\\Automation Test Result for Statutory Scenarios201718.xlsx</t>
-  </si>
-  <si>
     <t>TestReportWorksheetNo</t>
   </si>
   <si>
@@ -582,14 +584,16 @@
   </si>
   <si>
     <t>9</t>
+  </si>
+  <si>
+    <t>F:\\Automation_TestResults\\Payroll_Tax_StatutoryScenarios\\Automation Test Result for Statutory Scenarios201718.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -653,65 +657,68 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="21">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyProtection="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -722,10 +729,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -760,7 +767,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -793,9 +800,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -828,6 +852,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -883,7 +924,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -892,13 +933,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -908,7 +949,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -917,7 +958,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -926,7 +967,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -936,12 +977,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -972,7 +1013,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -991,7 +1032,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1003,22 +1044,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="32.44140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="44.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.33203125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.11328125" collapsed="true"/>
+    <col min="1" max="1" width="32.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="44.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1032,7 +1073,7 @@
         <v>3</v>
       </c>
     </row>
-    <row ht="28.8" r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>98</v>
       </c>
@@ -1046,7 +1087,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>129</v>
       </c>
@@ -1060,7 +1101,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -1074,7 +1115,7 @@
         <v>114</v>
       </c>
     </row>
-    <row ht="28.8" r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>103</v>
       </c>
@@ -1088,7 +1129,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>110</v>
       </c>
@@ -1102,7 +1143,7 @@
         <v>5</v>
       </c>
     </row>
-    <row ht="28.8" r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>154</v>
       </c>
@@ -1116,7 +1157,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>136</v>
       </c>
@@ -1130,7 +1171,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>155</v>
       </c>
@@ -1144,7 +1185,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>160</v>
       </c>
@@ -1158,7 +1199,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>156</v>
       </c>
@@ -1172,7 +1213,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>159</v>
       </c>
@@ -1186,7 +1227,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>133</v>
       </c>
@@ -1200,7 +1241,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>135</v>
       </c>
@@ -1214,7 +1255,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>157</v>
       </c>
@@ -1228,7 +1269,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>158</v>
       </c>
@@ -1243,32 +1284,32 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="35.5546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="10.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="28.109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="29.109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="28.5546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="21.33203125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.44140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="23.33203125" collapsed="true"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="28.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="36.42578125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>115</v>
       </c>
@@ -1300,7 +1341,7 @@
         <v>123</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>2</v>
@@ -1312,7 +1353,7 @@
         <v>66</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="62.4" r="2" s="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="19" customFormat="1" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>168</v>
       </c>
@@ -1333,48 +1374,48 @@
         <v>152</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J2" s="16" t="s">
         <v>124</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L2" s="18" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="35.5546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="34.77734375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="27.44140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="37.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.6640625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.33203125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="22.21875" collapsed="true"/>
+    <col min="1" max="1" width="35.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="27.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="37" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>115</v>
       </c>
@@ -1406,7 +1447,7 @@
         <v>123</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>2</v>
@@ -1418,7 +1459,7 @@
         <v>66</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="19" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>168</v>
       </c>
@@ -1432,7 +1473,7 @@
         <v>96</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F2" s="16" t="s">
         <v>171</v>
@@ -1441,7 +1482,7 @@
         <v>153</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="I2" s="16" t="s">
         <v>164</v>
@@ -1450,32 +1491,32 @@
         <v>124</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L2" s="18" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="42.33203125" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="1" max="1" width="42.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="18" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>97</v>
       </c>
@@ -1495,7 +1536,7 @@
         <v>66</v>
       </c>
     </row>
-    <row customHeight="1" ht="21.6" r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>148</v>
       </c>
@@ -1510,35 +1551,35 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BK2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="AR1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="27.5546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="27.6640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="24.88671875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.6640625" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="17.109375" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="24.6640625" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="15.109375" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="37" max="37" customWidth="true" width="15.44140625" collapsed="true"/>
-    <col min="38" max="38" customWidth="true" width="22.33203125" collapsed="true"/>
-    <col min="39" max="39" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="24.7109375" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="22.28515625" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="25" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1729,7 +1770,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>101</v>
       </c>
@@ -1916,29 +1957,29 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId3" ref="C2"/>
-    <hyperlink r:id="rId4" ref="D2"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="43.77734375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="24.88671875" collapsed="true"/>
+    <col min="1" max="1" width="43.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>97</v>
       </c>
@@ -1964,7 +2005,7 @@
         <v>66</v>
       </c>
     </row>
-    <row customHeight="1" ht="21.6" r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>148</v>
       </c>
@@ -1985,25 +2026,25 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="48.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="22.6640625" collapsed="true"/>
+    <col min="1" max="1" width="48.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>97</v>
       </c>
@@ -2020,7 +2061,7 @@
         <v>66</v>
       </c>
     </row>
-    <row customHeight="1" ht="17.399999999999999" r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>148</v>
       </c>
@@ -2032,36 +2073,36 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="35.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="35.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="14.109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.21875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.33203125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="26.109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="42.6640625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.88671875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="23.5546875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="11.109375" collapsed="true"/>
+    <col min="1" max="1" width="35.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="26.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="42.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.5703125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>115</v>
       </c>
@@ -2093,7 +2134,7 @@
         <v>123</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>2</v>
@@ -2105,7 +2146,7 @@
         <v>66</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="19" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>168</v>
       </c>
@@ -2128,7 +2169,7 @@
         <v>149</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="I2" s="16" t="s">
         <v>161</v>
@@ -2137,40 +2178,40 @@
         <v>124</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L2" s="18" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="35.5546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="34.109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.77734375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="40.109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="34.88671875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="39.44140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.44140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="21.21875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="5.6640625" collapsed="true"/>
+    <col min="1" max="1" width="35.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="40.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="34.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="39.42578125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="5.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>115</v>
       </c>
@@ -2202,7 +2243,7 @@
         <v>123</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>2</v>
@@ -2214,7 +2255,7 @@
         <v>66</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="19" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>168</v>
       </c>
@@ -2228,7 +2269,7 @@
         <v>96</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F2" s="16" t="s">
         <v>171</v>
@@ -2237,7 +2278,7 @@
         <v>149</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="I2" s="16" t="s">
         <v>162</v>
@@ -2246,38 +2287,38 @@
         <v>124</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L2" s="18" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="36.77734375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="35.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.21875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="28.6640625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="27.109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="38.109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="26.5546875" collapsed="true"/>
+    <col min="1" max="1" width="36.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="28.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="27.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="38.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="26.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>115</v>
       </c>
@@ -2309,7 +2350,7 @@
         <v>123</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>2</v>
@@ -2321,7 +2362,7 @@
         <v>66</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="19" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>168</v>
       </c>
@@ -2335,7 +2376,7 @@
         <v>96</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F2" s="16" t="s">
         <v>171</v>
@@ -2344,7 +2385,7 @@
         <v>149</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="I2" s="16" t="s">
         <v>163</v>
@@ -2353,39 +2394,39 @@
         <v>124</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L2" s="18" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="37.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="11.77734375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.77734375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="12.6640625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="12.5546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="38.6640625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="19.6640625" collapsed="true"/>
+    <col min="1" max="1" width="37.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="38.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>97</v>
       </c>
@@ -2423,27 +2464,27 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>148</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>150</v>
       </c>
       <c r="D2" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="E2" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="F2" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="G2" s="20" t="s">
         <v>179</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>180</v>
       </c>
       <c r="H2" s="10" t="s">
         <v>151</v>
@@ -2456,6 +2497,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Code Merge Changes- Xls files are updated - 9/25/2017
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite Statutory Adoption PaternityPay201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite Statutory Adoption PaternityPay201718.xlsx
@@ -586,7 +586,7 @@
     <t>9</t>
   </si>
   <si>
-    <t>F:\\Automation_TestResults\\Payroll_Tax_StatutoryScenarios\\Automation Test Result for Statutory Scenarios201718.xlsx</t>
+    <t>F:\\Automation_TestResults\\Payroll_Tax_StatutoryScenarios\\201718 Automation TestResult For Statutory Scenarios.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1293,7 +1293,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2194,7 +2194,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2303,7 +2303,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
committing SAPP Pagination work
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite Statutory Adoption PaternityPay201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite Statutory Adoption PaternityPay201718.xlsx
@@ -4,27 +4,27 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="396" yWindow="36" windowWidth="15168" windowHeight="5400" firstSheet="8" activeTab="10"/>
+    <workbookView activeTab="10" firstSheet="8" windowHeight="5400" windowWidth="15168" xWindow="396" yWindow="36"/>
   </bookViews>
   <sheets>
-    <sheet name="first" sheetId="1" r:id="rId1"/>
-    <sheet name="ResetData" sheetId="14" r:id="rId2"/>
-    <sheet name="CreateFemaleEmployee" sheetId="2" r:id="rId3"/>
-    <sheet name="UpdateTaxCodeAndAnnualSalary" sheetId="6" r:id="rId4"/>
-    <sheet name="SmallEmployerRelief" sheetId="3" r:id="rId5"/>
-    <sheet name="ProcessPayrollForJulyMonthSAPP" sheetId="7" r:id="rId6"/>
-    <sheet name="ProcessPayrollForAugMonthSAPP" sheetId="8" r:id="rId7"/>
-    <sheet name="ProcessPayrollForSepMonthSAPP" sheetId="9" r:id="rId8"/>
-    <sheet name="CreateLeaveRequest" sheetId="10" r:id="rId9"/>
-    <sheet name="AverageWeeklyEarningsTestReport" sheetId="11" r:id="rId10"/>
-    <sheet name="ProcessPayrollForJan16MonthSAPP" sheetId="12" r:id="rId11"/>
+    <sheet name="first" r:id="rId1" sheetId="1"/>
+    <sheet name="ResetData" r:id="rId2" sheetId="14"/>
+    <sheet name="CreateFemaleEmployee" r:id="rId3" sheetId="2"/>
+    <sheet name="UpdateTaxCodeAndAnnualSalary" r:id="rId4" sheetId="6"/>
+    <sheet name="SmallEmployerRelief" r:id="rId5" sheetId="3"/>
+    <sheet name="ProcessPayrollForJulyMonthSAPP" r:id="rId6" sheetId="7"/>
+    <sheet name="ProcessPayrollForAugMonthSAPP" r:id="rId7" sheetId="8"/>
+    <sheet name="ProcessPayrollForSepMonthSAPP" r:id="rId8" sheetId="9"/>
+    <sheet name="CreateLeaveRequest" r:id="rId9" sheetId="10"/>
+    <sheet name="AverageWeeklyEarningsTestReport" r:id="rId10" sheetId="11"/>
+    <sheet name="ProcessPayrollForJan16MonthSAPP" r:id="rId11" sheetId="12"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="186">
   <si>
     <t>TC</t>
   </si>
@@ -588,6 +588,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -652,63 +653,63 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="22">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyProtection="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="2">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -725,10 +726,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -886,7 +887,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -895,13 +896,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -911,7 +912,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -920,7 +921,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -929,7 +930,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -939,12 +940,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -975,7 +976,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -994,7 +995,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1006,7 +1007,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1015,13 +1016,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="44.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="44.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.11328125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1035,7 +1036,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>98</v>
       </c>
@@ -1049,7 +1050,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>129</v>
       </c>
@@ -1063,7 +1064,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -1077,7 +1078,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>103</v>
       </c>
@@ -1091,7 +1092,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>110</v>
       </c>
@@ -1105,7 +1106,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>154</v>
       </c>
@@ -1119,7 +1120,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>136</v>
       </c>
@@ -1133,7 +1134,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>155</v>
       </c>
@@ -1147,7 +1148,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>160</v>
       </c>
@@ -1161,7 +1162,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>156</v>
       </c>
@@ -1246,12 +1247,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -1260,18 +1261,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="35.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.5546875" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="36.44140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21.33203125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.44140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="35.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.5546875" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="28.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="36.44140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="21.33203125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.44140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>115</v>
       </c>
@@ -1315,7 +1316,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="19" customFormat="1" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="62.4" r="2" s="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>183</v>
       </c>
@@ -1353,14 +1354,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
@@ -1369,19 +1370,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="37" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.44140625" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.44140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="37.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>115</v>
       </c>
@@ -1425,7 +1426,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="19" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>183</v>
       </c>
@@ -1465,14 +1466,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1481,11 +1482,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="18" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="42.33203125" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="18.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>97</v>
       </c>
@@ -1505,7 +1506,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="21.6" r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>148</v>
       </c>
@@ -1520,12 +1521,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BK2"/>
   <sheetViews>
     <sheetView topLeftCell="AR1" workbookViewId="0">
@@ -1534,18 +1535,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="17.109375" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="24.6640625" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="15.109375" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="15.44140625" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="22.33203125" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="25" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="24.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.6640625" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="17.109375" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="24.6640625" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="37" max="37" customWidth="true" width="15.44140625" collapsed="true"/>
+    <col min="38" max="38" customWidth="true" width="22.33203125" collapsed="true"/>
+    <col min="39" max="39" customWidth="true" width="25.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:63" x14ac:dyDescent="0.25">
@@ -1926,15 +1927,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink r:id="rId1" ref="C2"/>
+    <hyperlink r:id="rId2" ref="D2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1943,12 +1944,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="43.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="24.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>97</v>
       </c>
@@ -1974,7 +1975,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="21.6" r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>148</v>
       </c>
@@ -1995,12 +1996,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2009,11 +2010,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="48.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>97</v>
       </c>
@@ -2030,7 +2031,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="17.399999999999999" r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>148</v>
       </c>
@@ -2042,13 +2043,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -2057,21 +2058,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.88671875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42.6640625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.88671875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.5546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.88671875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.5546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>115</v>
       </c>
@@ -2115,7 +2116,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="19" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>183</v>
       </c>
@@ -2155,14 +2156,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -2171,19 +2172,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="40.109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.88671875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="39.44140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.44140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="21.33203125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="5.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="40.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.88671875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="39.44140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.44140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="21.33203125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="5.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>115</v>
       </c>
@@ -2227,7 +2228,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="19" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>183</v>
       </c>
@@ -2267,14 +2268,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -2283,18 +2284,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.21875" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.6640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="38.109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="26.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="36.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.21875" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="28.6640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="38.109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="26.5546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>115</v>
       </c>
@@ -2338,7 +2339,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="19" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>183</v>
       </c>
@@ -2378,14 +2379,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2394,15 +2395,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.5546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="38.6640625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="38.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="19.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -2476,6 +2477,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>